<commit_message>
put all constants at the top
</commit_message>
<xml_diff>
--- a/api_allocate.xlsx
+++ b/api_allocate.xlsx
@@ -112,9 +112,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
@@ -507,14 +507,14 @@
     <col width="6" customWidth="1" min="2" max="2"/>
     <col width="20" customWidth="1" min="3" max="3"/>
     <col width="20" customWidth="1" min="4" max="4"/>
-    <col width="24" customWidth="1" min="5" max="5"/>
+    <col width="19" customWidth="1" min="5" max="5"/>
     <col width="21" customWidth="1" min="6" max="6"/>
-    <col width="21" customWidth="1" min="7" max="7"/>
+    <col width="24" customWidth="1" min="7" max="7"/>
     <col width="46" customWidth="1" min="10" max="10"/>
-    <col width="24" customWidth="1" min="11" max="11"/>
-    <col width="20" customWidth="1" min="12" max="12"/>
-    <col width="20" customWidth="1" min="13" max="13"/>
-    <col width="107" customWidth="1" min="14" max="14"/>
+    <col width="20" customWidth="1" min="11" max="11"/>
+    <col width="19" customWidth="1" min="12" max="12"/>
+    <col width="103" customWidth="1" min="13" max="13"/>
+    <col width="20" customWidth="1" min="14" max="14"/>
     <col width="21" customWidth="1" min="15" max="15"/>
   </cols>
   <sheetData>
@@ -557,27 +557,27 @@
       </c>
       <c r="K2" s="5" t="inlineStr">
         <is>
+          <t>Driver: Clay Murphy</t>
+        </is>
+      </c>
+      <c r="L2" s="5" t="inlineStr">
+        <is>
+          <t>Driver: Ellie Jung</t>
+        </is>
+      </c>
+      <c r="M2" s="5" t="inlineStr">
+        <is>
+          <t>Driver: Olivia Chang</t>
+        </is>
+      </c>
+      <c r="N2" s="5" t="inlineStr">
+        <is>
+          <t>Driver: david kim</t>
+        </is>
+      </c>
+      <c r="O2" s="5" t="inlineStr">
+        <is>
           <t>Driver: Josh Paik</t>
-        </is>
-      </c>
-      <c r="L2" s="5" t="inlineStr">
-        <is>
-          <t>Driver: Clay Murphy</t>
-        </is>
-      </c>
-      <c r="M2" s="5" t="inlineStr">
-        <is>
-          <t>Driver: Ellie Jung</t>
-        </is>
-      </c>
-      <c r="N2" s="5" t="inlineStr">
-        <is>
-          <t>Driver: Brian Seo</t>
-        </is>
-      </c>
-      <c r="O2" s="5" t="inlineStr">
-        <is>
-          <t>Driver: Olivia Chang</t>
         </is>
       </c>
     </row>
@@ -589,228 +589,228 @@
       </c>
       <c r="C3" s="1" t="inlineStr">
         <is>
+          <t>Aaron Long</t>
+        </is>
+      </c>
+      <c r="D3" s="1" t="inlineStr">
+        <is>
+          <t>JJ Lee</t>
+        </is>
+      </c>
+      <c r="E3" s="1" t="inlineStr">
+        <is>
           <t>Sehyun Jung</t>
         </is>
       </c>
-      <c r="D3" s="1" t="inlineStr">
+      <c r="F3" s="7" t="inlineStr">
+        <is>
+          <t>Jacob Lei</t>
+        </is>
+      </c>
+      <c r="G3" s="6" t="inlineStr">
+        <is>
+          <t>Susanna Tang</t>
+        </is>
+      </c>
+      <c r="J3" s="8" t="inlineStr">
+        <is>
+          <t>Lunch 💛</t>
+        </is>
+      </c>
+      <c r="K3" s="1" t="inlineStr">
+        <is>
+          <t>Nathanael Wang</t>
+        </is>
+      </c>
+      <c r="L3" s="1" t="inlineStr">
+        <is>
+          <t>JJ Lee</t>
+        </is>
+      </c>
+      <c r="M3" s="6" t="inlineStr">
+        <is>
+          <t>Sabrina Sun</t>
+        </is>
+      </c>
+      <c r="N3" s="6" t="inlineStr">
+        <is>
+          <t>Logan Golia</t>
+        </is>
+      </c>
+      <c r="O3" s="7" t="inlineStr">
+        <is>
+          <t>Jane Yoo</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" s="7" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="C4" s="1" t="inlineStr">
+        <is>
+          <t>Grace Park</t>
+        </is>
+      </c>
+      <c r="D4" s="1" t="inlineStr">
+        <is>
+          <t>Christina Ko</t>
+        </is>
+      </c>
+      <c r="E4" s="7" t="inlineStr">
+        <is>
+          <t>Faith Chen</t>
+        </is>
+      </c>
+      <c r="F4" s="9" t="inlineStr">
+        <is>
+          <t>Claire Doh</t>
+        </is>
+      </c>
+      <c r="G4" s="6" t="inlineStr">
+        <is>
+          <t>Josh Yang</t>
+        </is>
+      </c>
+      <c r="J4" s="10" t="inlineStr">
+        <is>
+          <t>Refreshments 💜 (Phnom Penh &amp; Albania HC only)</t>
+        </is>
+      </c>
+      <c r="K4" s="1" t="inlineStr">
+        <is>
+          <t>chloe lim</t>
+        </is>
+      </c>
+      <c r="L4" s="6" t="inlineStr">
+        <is>
+          <t>Josh Yang</t>
+        </is>
+      </c>
+      <c r="M4" s="7" t="inlineStr">
+        <is>
+          <t>claudia lin</t>
+        </is>
+      </c>
+      <c r="N4" s="6" t="inlineStr">
+        <is>
+          <t>Susanna Tang</t>
+        </is>
+      </c>
+      <c r="O4" s="7" t="inlineStr">
+        <is>
+          <t>Jacob Lei</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" s="9" t="inlineStr">
+        <is>
+          <t>South</t>
+        </is>
+      </c>
+      <c r="C5" s="1" t="inlineStr">
+        <is>
+          <t>chloe lim</t>
+        </is>
+      </c>
+      <c r="D5" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">Michael Dong </t>
         </is>
       </c>
-      <c r="E3" s="1" t="inlineStr">
-        <is>
-          <t>Christina Ko</t>
-        </is>
-      </c>
-      <c r="F3" s="7" t="inlineStr">
-        <is>
-          <t>Claire Doh</t>
-        </is>
-      </c>
-      <c r="G3" s="6" t="inlineStr">
-        <is>
-          <t>Susanna Tang</t>
-        </is>
-      </c>
-      <c r="J3" s="8" t="inlineStr">
-        <is>
-          <t>Lunch 💛</t>
-        </is>
-      </c>
-      <c r="K3" s="9" t="inlineStr">
-        <is>
-          <t>Jeff Jiang</t>
-        </is>
-      </c>
-      <c r="L3" s="6" t="inlineStr">
+      <c r="E5" s="7" t="inlineStr">
+        <is>
+          <t>claudia lin</t>
+        </is>
+      </c>
+      <c r="F5" s="9" t="inlineStr">
+        <is>
+          <t>David Zhu</t>
+        </is>
+      </c>
+      <c r="G5" s="6" t="inlineStr">
+        <is>
+          <t>Jocelyn Youn</t>
+        </is>
+      </c>
+      <c r="K5" s="1" t="inlineStr">
+        <is>
+          <t>Sehyun Jung</t>
+        </is>
+      </c>
+      <c r="L5" s="6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Daniel Kim </t>
+        </is>
+      </c>
+      <c r="M5" s="7" t="inlineStr">
+        <is>
+          <t>Faith Chen</t>
+        </is>
+      </c>
+      <c r="N5" s="6" t="inlineStr">
         <is>
           <t>Daniel Song</t>
         </is>
       </c>
-      <c r="M3" s="6" t="inlineStr">
-        <is>
-          <t>Logan Golia</t>
-        </is>
-      </c>
-      <c r="N3" s="7" t="inlineStr">
-        <is>
-          <t>Daniel Kuo</t>
-        </is>
-      </c>
-      <c r="O3" s="7" t="inlineStr">
-        <is>
-          <t>Israel Haile</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="B4" s="9" t="inlineStr">
-        <is>
-          <t>Off</t>
-        </is>
-      </c>
-      <c r="C4" s="1" t="inlineStr">
-        <is>
-          <t>Grace Park</t>
-        </is>
-      </c>
-      <c r="D4" s="1" t="inlineStr">
-        <is>
-          <t>Phillip Seo</t>
-        </is>
-      </c>
-      <c r="E4" s="9" t="inlineStr">
-        <is>
-          <t>Faith Chen</t>
-        </is>
-      </c>
-      <c r="F4" s="7" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Derek Liang </t>
-        </is>
-      </c>
-      <c r="G4" s="6" t="inlineStr">
-        <is>
-          <t>Sabrina Sun</t>
-        </is>
-      </c>
-      <c r="J4" s="10" t="inlineStr">
-        <is>
-          <t>Refreshments 💜 (Phnom Penh &amp; Albania HC only)</t>
-        </is>
-      </c>
-      <c r="K4" s="7" t="inlineStr">
-        <is>
-          <t>Hannah Kim</t>
-        </is>
-      </c>
-      <c r="L4" s="6" t="inlineStr">
-        <is>
-          <t>Sabrina Sun</t>
-        </is>
-      </c>
-      <c r="M4" s="6" t="inlineStr">
-        <is>
-          <t>Susanna Tang</t>
-        </is>
-      </c>
-      <c r="N4" s="7" t="inlineStr">
+      <c r="O5" s="9" t="inlineStr">
         <is>
           <t>Rachel Kim</t>
-        </is>
-      </c>
-      <c r="O4" s="7" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Derek Liang </t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="B5" s="7" t="inlineStr">
-        <is>
-          <t>South</t>
-        </is>
-      </c>
-      <c r="C5" s="1" t="inlineStr">
-        <is>
-          <t>JJ Lee</t>
-        </is>
-      </c>
-      <c r="D5" s="1" t="inlineStr">
-        <is>
-          <t>Nathanael Wang</t>
-        </is>
-      </c>
-      <c r="E5" s="9" t="inlineStr">
-        <is>
-          <t>claudia lin</t>
-        </is>
-      </c>
-      <c r="F5" s="7" t="inlineStr">
-        <is>
-          <t>Hannah Kim</t>
-        </is>
-      </c>
-      <c r="G5" s="6" t="inlineStr">
-        <is>
-          <t>Jocelyn Youn</t>
-        </is>
-      </c>
-      <c r="K5" s="7" t="inlineStr">
-        <is>
-          <t>Grace Kwon</t>
-        </is>
-      </c>
-      <c r="L5" s="6" t="inlineStr">
-        <is>
-          <t>Samuel Wen</t>
-        </is>
-      </c>
-      <c r="M5" s="6" t="inlineStr">
-        <is>
-          <t>Josh Yang</t>
-        </is>
-      </c>
-      <c r="N5" s="7" t="inlineStr">
-        <is>
-          <t>Jiwang Lee</t>
-        </is>
-      </c>
-      <c r="O5" s="7" t="inlineStr">
-        <is>
-          <t>David Zhu</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="C6" s="1" t="inlineStr">
         <is>
-          <t>Aaron Long</t>
+          <t>Nathanael Wang</t>
         </is>
       </c>
       <c r="D6" s="1" t="inlineStr">
         <is>
-          <t>chloe lim</t>
-        </is>
-      </c>
-      <c r="E6" s="7" t="inlineStr">
-        <is>
-          <t>Benjamin Kim</t>
-        </is>
-      </c>
-      <c r="F6" s="7" t="inlineStr">
+          <t>Phillip Seo</t>
+        </is>
+      </c>
+      <c r="E6" s="9" t="inlineStr">
         <is>
           <t>Jeffery Huang</t>
         </is>
       </c>
+      <c r="F6" s="9" t="inlineStr">
+        <is>
+          <t>Daniel Kuo</t>
+        </is>
+      </c>
       <c r="G6" s="6" t="inlineStr">
         <is>
+          <t>Logan Golia</t>
+        </is>
+      </c>
+      <c r="K6" s="1" t="inlineStr">
+        <is>
+          <t>Christina Ko</t>
+        </is>
+      </c>
+      <c r="L6" s="6" t="inlineStr">
+        <is>
           <t>Samuel Wen</t>
         </is>
       </c>
-      <c r="K6" s="7" t="inlineStr">
-        <is>
-          <t>Jeffery Huang</t>
-        </is>
-      </c>
-      <c r="L6" s="6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Daniel Kim </t>
-        </is>
-      </c>
       <c r="M6" s="9" t="inlineStr">
         <is>
-          <t>Jacob Lei</t>
+          <t>Grace Kwon</t>
         </is>
       </c>
       <c r="N6" s="7" t="inlineStr">
         <is>
+          <t>Rebecca Lu</t>
+        </is>
+      </c>
+      <c r="O6" s="9" t="inlineStr">
+        <is>
           <t>Claire Doh</t>
-        </is>
-      </c>
-      <c r="O6" s="7" t="inlineStr">
-        <is>
-          <t>Joann Jung</t>
         </is>
       </c>
     </row>
@@ -824,34 +824,34 @@
       </c>
       <c r="D9" s="11" t="inlineStr">
         <is>
+          <t>Driver: Josh Paik</t>
+        </is>
+      </c>
+      <c r="E9" s="11" t="inlineStr">
+        <is>
           <t>Driver: david kim</t>
         </is>
       </c>
-      <c r="E9" s="11" t="inlineStr">
+      <c r="F9" s="11" t="inlineStr">
+        <is>
+          <t>Driver: Lia Kim</t>
+        </is>
+      </c>
+      <c r="G9" s="11" t="inlineStr">
         <is>
           <t>Driver: Jacob Deadlifts</t>
         </is>
       </c>
-      <c r="F9" s="11" t="inlineStr">
-        <is>
-          <t>Driver: Josh Paik</t>
-        </is>
-      </c>
-      <c r="G9" s="11" t="inlineStr">
+      <c r="K9" s="5" t="inlineStr">
+        <is>
+          <t>Driver: Brian Seo</t>
+        </is>
+      </c>
+      <c r="L9" s="5" t="inlineStr">
         <is>
           <t>Driver: Lia Kim</t>
         </is>
       </c>
-      <c r="K9" s="5" t="inlineStr">
-        <is>
-          <t>Driver: david kim</t>
-        </is>
-      </c>
-      <c r="L9" s="5" t="inlineStr">
-        <is>
-          <t>Driver: Lia Kim</t>
-        </is>
-      </c>
       <c r="M9" s="5" t="inlineStr">
         <is>
           <t>Driver: Oriana Tang</t>
@@ -859,180 +859,185 @@
       </c>
       <c r="N9" s="12" t="inlineStr">
         <is>
+          <t>Driver: Jocelyn Lee</t>
+        </is>
+      </c>
+      <c r="O9" s="12" t="inlineStr">
+        <is>
           <t>Driver: Jonathan Mak</t>
         </is>
       </c>
-      <c r="O9" s="12" t="inlineStr">
-        <is>
-          <t>Driver: Jocelyn Lee</t>
-        </is>
-      </c>
     </row>
     <row r="10">
-      <c r="C10" s="9" t="inlineStr">
+      <c r="C10" s="7" t="inlineStr">
+        <is>
+          <t>Rebecca Lu</t>
+        </is>
+      </c>
+      <c r="D10" s="7" t="inlineStr">
+        <is>
+          <t>Jane Yoo</t>
+        </is>
+      </c>
+      <c r="E10" s="9" t="inlineStr">
+        <is>
+          <t>Grace Kwon</t>
+        </is>
+      </c>
+      <c r="F10" s="6" t="inlineStr">
+        <is>
+          <t>Daniel Song</t>
+        </is>
+      </c>
+      <c r="G10" s="6" t="inlineStr">
+        <is>
+          <t>Sabrina Sun</t>
+        </is>
+      </c>
+      <c r="K10" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Derek Liang </t>
+        </is>
+      </c>
+      <c r="L10" s="9" t="inlineStr">
+        <is>
+          <t>Daniel Kuo</t>
+        </is>
+      </c>
+      <c r="M10" s="7" t="inlineStr">
+        <is>
+          <t>Jeff Jiang</t>
+        </is>
+      </c>
+      <c r="N10" s="1" t="inlineStr">
+        <is>
+          <t>Phillip Seo</t>
+        </is>
+      </c>
+      <c r="O10" s="6" t="inlineStr">
+        <is>
+          <t>Justin Zhang</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="D11" s="7" t="inlineStr">
+        <is>
+          <t>Austin Lee</t>
+        </is>
+      </c>
+      <c r="E11" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Derek Liang </t>
+        </is>
+      </c>
+      <c r="F11" s="6" t="inlineStr">
+        <is>
+          <t>Justin Zhang</t>
+        </is>
+      </c>
+      <c r="G11" s="6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Daniel Kim </t>
+        </is>
+      </c>
+      <c r="K11" s="9" t="inlineStr">
+        <is>
+          <t>Jeffery Huang</t>
+        </is>
+      </c>
+      <c r="L11" s="9" t="inlineStr">
+        <is>
+          <t>Joann Jung</t>
+        </is>
+      </c>
+      <c r="N11" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Michael Dong </t>
+        </is>
+      </c>
+      <c r="O11" s="6" t="inlineStr">
+        <is>
+          <t>Jocelyn Youn</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="D12" s="7" t="inlineStr">
         <is>
           <t>Seojin Kwon</t>
         </is>
       </c>
-      <c r="D10" s="6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Daniel Kim </t>
-        </is>
-      </c>
-      <c r="E10" s="6" t="inlineStr">
-        <is>
-          <t>Daniel Song</t>
-        </is>
-      </c>
-      <c r="F10" s="9" t="inlineStr">
-        <is>
-          <t>Jane Yoo</t>
-        </is>
-      </c>
-      <c r="G10" s="6" t="inlineStr">
-        <is>
-          <t>Logan Golia</t>
-        </is>
-      </c>
-      <c r="K10" s="9" t="inlineStr">
-        <is>
-          <t>Jane Yoo</t>
-        </is>
-      </c>
-      <c r="L10" s="1" t="inlineStr">
-        <is>
-          <t>chloe lim</t>
-        </is>
-      </c>
-      <c r="M10" s="1" t="inlineStr">
-        <is>
-          <t>Sehyun Jung</t>
-        </is>
-      </c>
-      <c r="N10" s="6" t="inlineStr">
-        <is>
-          <t>Justin Zhang</t>
-        </is>
-      </c>
-      <c r="O10" s="1" t="inlineStr">
+      <c r="E12" s="9" t="inlineStr">
+        <is>
+          <t>Joann Jung</t>
+        </is>
+      </c>
+      <c r="F12" s="6" t="inlineStr">
+        <is>
+          <t>Samuel Wen</t>
+        </is>
+      </c>
+      <c r="G12" s="7" t="inlineStr">
+        <is>
+          <t>Sam Ko</t>
+        </is>
+      </c>
+      <c r="K12" s="9" t="inlineStr">
+        <is>
+          <t>Hannah Kim</t>
+        </is>
+      </c>
+      <c r="L12" s="9" t="inlineStr">
+        <is>
+          <t>Jiwang Lee</t>
+        </is>
+      </c>
+      <c r="N12" s="1" t="inlineStr">
         <is>
           <t>Aaron Long</t>
         </is>
       </c>
-    </row>
-    <row r="11">
-      <c r="D11" s="9" t="inlineStr">
-        <is>
-          <t>Rebecca Lu</t>
-        </is>
-      </c>
-      <c r="E11" s="6" t="inlineStr">
-        <is>
-          <t>Justin Zhang</t>
-        </is>
-      </c>
-      <c r="F11" s="9" t="inlineStr">
+      <c r="O12" s="9" t="inlineStr">
+        <is>
+          <t>Benjamin Kim</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="D13" s="7" t="inlineStr">
+        <is>
+          <t>Khang Le</t>
+        </is>
+      </c>
+      <c r="E13" s="9" t="inlineStr">
+        <is>
+          <t>Benjamin Kim</t>
+        </is>
+      </c>
+      <c r="F13" s="9" t="inlineStr">
+        <is>
+          <t>Kyle Hwang</t>
+        </is>
+      </c>
+      <c r="G13" s="7" t="inlineStr">
+        <is>
+          <t>Jeff Jiang</t>
+        </is>
+      </c>
+      <c r="K13" s="9" t="inlineStr">
+        <is>
+          <t>David Zhu</t>
+        </is>
+      </c>
+      <c r="L13" s="9" t="inlineStr">
+        <is>
+          <t>Israel Haile</t>
+        </is>
+      </c>
+      <c r="N13" s="7" t="inlineStr">
         <is>
           <t>Austin Lee</t>
-        </is>
-      </c>
-      <c r="G11" s="7" t="inlineStr">
-        <is>
-          <t>Kyle Hwang</t>
-        </is>
-      </c>
-      <c r="K11" s="9" t="inlineStr">
-        <is>
-          <t>Rebecca Lu</t>
-        </is>
-      </c>
-      <c r="L11" s="1" t="inlineStr">
-        <is>
-          <t>JJ Lee</t>
-        </is>
-      </c>
-      <c r="N11" s="6" t="inlineStr">
-        <is>
-          <t>Jocelyn Youn</t>
-        </is>
-      </c>
-      <c r="O11" s="1" t="inlineStr">
-        <is>
-          <t>Phillip Seo</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="D12" s="9" t="inlineStr">
-        <is>
-          <t>Jeff Jiang</t>
-        </is>
-      </c>
-      <c r="E12" s="6" t="inlineStr">
-        <is>
-          <t>Josh Yang</t>
-        </is>
-      </c>
-      <c r="F12" s="9" t="inlineStr">
-        <is>
-          <t>Jacob Lei</t>
-        </is>
-      </c>
-      <c r="G12" s="7" t="inlineStr">
-        <is>
-          <t>Taeho Choe</t>
-        </is>
-      </c>
-      <c r="K12" s="9" t="inlineStr">
-        <is>
-          <t>Faith Chen</t>
-        </is>
-      </c>
-      <c r="L12" s="1" t="inlineStr">
-        <is>
-          <t>Nathanael Wang</t>
-        </is>
-      </c>
-      <c r="O12" s="9" t="inlineStr">
-        <is>
-          <t>Austin Lee</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="D13" s="9" t="inlineStr">
-        <is>
-          <t>Sam Ko</t>
-        </is>
-      </c>
-      <c r="E13" s="9" t="inlineStr">
-        <is>
-          <t>Khang Le</t>
-        </is>
-      </c>
-      <c r="F13" s="7" t="inlineStr">
-        <is>
-          <t>Joann Jung</t>
-        </is>
-      </c>
-      <c r="G13" s="7" t="inlineStr">
-        <is>
-          <t>Jiwang Lee</t>
-        </is>
-      </c>
-      <c r="K13" s="9" t="inlineStr">
-        <is>
-          <t>claudia lin</t>
-        </is>
-      </c>
-      <c r="L13" s="1" t="inlineStr">
-        <is>
-          <t>Christina Ko</t>
-        </is>
-      </c>
-      <c r="O13" s="7" t="inlineStr">
-        <is>
-          <t>Benjamin Kim</t>
         </is>
       </c>
     </row>
@@ -1049,85 +1054,75 @@
           <t>Driver: Oriana Tang</t>
         </is>
       </c>
-      <c r="K16" s="12" t="inlineStr">
-        <is>
-          <t>Driver: Jacob Deadlifts</t>
-        </is>
-      </c>
-      <c r="L16" s="14" t="inlineStr">
+      <c r="K16" s="14" t="inlineStr">
         <is>
           <t>Driver: Matthew Ahn</t>
         </is>
       </c>
-      <c r="N16" s="15" t="inlineStr">
+      <c r="M16" s="15" t="inlineStr">
         <is>
           <t>UNASSIGNED RIDERS</t>
         </is>
       </c>
     </row>
     <row r="17">
-      <c r="C17" s="7" t="inlineStr">
+      <c r="C17" s="9" t="inlineStr">
+        <is>
+          <t>Jiwang Lee</t>
+        </is>
+      </c>
+      <c r="D17" s="9" t="inlineStr">
+        <is>
+          <t>Rachel Kim</t>
+        </is>
+      </c>
+      <c r="K17" s="1" t="inlineStr">
+        <is>
+          <t>Grace Park</t>
+        </is>
+      </c>
+      <c r="M17" s="7" t="inlineStr">
+        <is>
+          <t>Sam Ko (Refreshments 💜 (Phnom Penh &amp; Albania HC only)) No valid driver available to assign this driver</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="C18" s="9" t="inlineStr">
         <is>
           <t>Israel Haile</t>
         </is>
       </c>
-      <c r="D17" s="7" t="inlineStr">
-        <is>
-          <t>Rachel Kim</t>
-        </is>
-      </c>
-      <c r="K17" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Michael Dong </t>
-        </is>
-      </c>
-      <c r="L17" s="9" t="inlineStr">
-        <is>
-          <t>Sam Ko</t>
-        </is>
-      </c>
-      <c r="N17" s="1" t="inlineStr">
-        <is>
-          <t>Grace Park (Refreshments 💜 (Phnom Penh &amp; Albania HC only)) No valid driver available to assign this driver</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="C18" s="7" t="inlineStr">
-        <is>
-          <t>Daniel Kuo</t>
-        </is>
-      </c>
-      <c r="L18" s="9" t="inlineStr">
+      <c r="K18" s="7" t="inlineStr">
         <is>
           <t>Khang Le</t>
         </is>
       </c>
-      <c r="N18" s="9" t="inlineStr">
+      <c r="M18" s="7" t="inlineStr">
         <is>
           <t>Seojin Kwon (NLK 🧡) No valid driver available to assign this driver</t>
         </is>
       </c>
     </row>
     <row r="19">
-      <c r="C19" s="7" t="inlineStr">
-        <is>
-          <t>David Zhu</t>
-        </is>
-      </c>
-      <c r="L19" s="7" t="inlineStr">
+      <c r="C19" s="9" t="inlineStr">
         <is>
           <t>Taeho Choe</t>
         </is>
       </c>
+      <c r="K19" s="9" t="inlineStr">
+        <is>
+          <t>Taeho Choe</t>
+        </is>
+      </c>
     </row>
     <row r="20">
-      <c r="C20" s="7" t="inlineStr">
-        <is>
-          <t>Grace Kwon</t>
-        </is>
-      </c>
-      <c r="L20" s="7" t="inlineStr">
+      <c r="C20" s="9" t="inlineStr">
+        <is>
+          <t>Hannah Kim</t>
+        </is>
+      </c>
+      <c r="K20" s="9" t="inlineStr">
         <is>
           <t>Kyle Hwang</t>
         </is>

</xml_diff>

<commit_message>
constants to the top
</commit_message>
<xml_diff>
--- a/api_allocate.xlsx
+++ b/api_allocate.xlsx
@@ -589,52 +589,52 @@
       </c>
       <c r="C3" s="1" t="inlineStr">
         <is>
-          <t>Aaron Long</t>
+          <t>Nathanael Wang</t>
         </is>
       </c>
       <c r="D3" s="1" t="inlineStr">
         <is>
+          <t>Grace Park</t>
+        </is>
+      </c>
+      <c r="E3" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Michael Dong </t>
+        </is>
+      </c>
+      <c r="F3" s="7" t="inlineStr">
+        <is>
+          <t>Jacob Lei</t>
+        </is>
+      </c>
+      <c r="G3" s="6" t="inlineStr">
+        <is>
+          <t>Josh Yang</t>
+        </is>
+      </c>
+      <c r="J3" s="8" t="inlineStr">
+        <is>
+          <t>Lunch 💛</t>
+        </is>
+      </c>
+      <c r="K3" s="1" t="inlineStr">
+        <is>
+          <t>chloe lim</t>
+        </is>
+      </c>
+      <c r="L3" s="1" t="inlineStr">
+        <is>
           <t>JJ Lee</t>
         </is>
       </c>
-      <c r="E3" s="1" t="inlineStr">
-        <is>
-          <t>Sehyun Jung</t>
-        </is>
-      </c>
-      <c r="F3" s="7" t="inlineStr">
-        <is>
-          <t>Jacob Lei</t>
-        </is>
-      </c>
-      <c r="G3" s="6" t="inlineStr">
-        <is>
-          <t>Susanna Tang</t>
-        </is>
-      </c>
-      <c r="J3" s="8" t="inlineStr">
-        <is>
-          <t>Lunch 💛</t>
-        </is>
-      </c>
-      <c r="K3" s="1" t="inlineStr">
-        <is>
-          <t>Nathanael Wang</t>
-        </is>
-      </c>
-      <c r="L3" s="1" t="inlineStr">
-        <is>
-          <t>JJ Lee</t>
-        </is>
-      </c>
       <c r="M3" s="6" t="inlineStr">
         <is>
+          <t>Samuel Wen</t>
+        </is>
+      </c>
+      <c r="N3" s="6" t="inlineStr">
+        <is>
           <t>Sabrina Sun</t>
-        </is>
-      </c>
-      <c r="N3" s="6" t="inlineStr">
-        <is>
-          <t>Logan Golia</t>
         </is>
       </c>
       <c r="O3" s="7" t="inlineStr">
@@ -651,12 +651,12 @@
       </c>
       <c r="C4" s="1" t="inlineStr">
         <is>
-          <t>Grace Park</t>
+          <t>Christina Ko</t>
         </is>
       </c>
       <c r="D4" s="1" t="inlineStr">
         <is>
-          <t>Christina Ko</t>
+          <t>Phillip Seo</t>
         </is>
       </c>
       <c r="E4" s="7" t="inlineStr">
@@ -666,37 +666,37 @@
       </c>
       <c r="F4" s="9" t="inlineStr">
         <is>
-          <t>Claire Doh</t>
+          <t>Daniel Kuo</t>
         </is>
       </c>
       <c r="G4" s="6" t="inlineStr">
         <is>
+          <t>Susanna Tang</t>
+        </is>
+      </c>
+      <c r="J4" s="10" t="inlineStr">
+        <is>
+          <t>Refreshments 💜 (Phnom Penh &amp; Albania HC only)</t>
+        </is>
+      </c>
+      <c r="K4" s="1" t="inlineStr">
+        <is>
+          <t>Sehyun Jung</t>
+        </is>
+      </c>
+      <c r="L4" s="6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Daniel Kim </t>
+        </is>
+      </c>
+      <c r="M4" s="7" t="inlineStr">
+        <is>
+          <t>Faith Chen</t>
+        </is>
+      </c>
+      <c r="N4" s="6" t="inlineStr">
+        <is>
           <t>Josh Yang</t>
-        </is>
-      </c>
-      <c r="J4" s="10" t="inlineStr">
-        <is>
-          <t>Refreshments 💜 (Phnom Penh &amp; Albania HC only)</t>
-        </is>
-      </c>
-      <c r="K4" s="1" t="inlineStr">
-        <is>
-          <t>chloe lim</t>
-        </is>
-      </c>
-      <c r="L4" s="6" t="inlineStr">
-        <is>
-          <t>Josh Yang</t>
-        </is>
-      </c>
-      <c r="M4" s="7" t="inlineStr">
-        <is>
-          <t>claudia lin</t>
-        </is>
-      </c>
-      <c r="N4" s="6" t="inlineStr">
-        <is>
-          <t>Susanna Tang</t>
         </is>
       </c>
       <c r="O4" s="7" t="inlineStr">
@@ -713,14 +713,14 @@
       </c>
       <c r="C5" s="1" t="inlineStr">
         <is>
+          <t>Sehyun Jung</t>
+        </is>
+      </c>
+      <c r="D5" s="1" t="inlineStr">
+        <is>
           <t>chloe lim</t>
         </is>
       </c>
-      <c r="D5" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Michael Dong </t>
-        </is>
-      </c>
       <c r="E5" s="7" t="inlineStr">
         <is>
           <t>claudia lin</t>
@@ -728,27 +728,27 @@
       </c>
       <c r="F5" s="9" t="inlineStr">
         <is>
-          <t>David Zhu</t>
+          <t>Kyle Hwang</t>
         </is>
       </c>
       <c r="G5" s="6" t="inlineStr">
         <is>
-          <t>Jocelyn Youn</t>
+          <t>Sabrina Sun</t>
         </is>
       </c>
       <c r="K5" s="1" t="inlineStr">
         <is>
-          <t>Sehyun Jung</t>
+          <t>Christina Ko</t>
         </is>
       </c>
       <c r="L5" s="6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Daniel Kim </t>
+          <t>Susanna Tang</t>
         </is>
       </c>
       <c r="M5" s="7" t="inlineStr">
         <is>
-          <t>Faith Chen</t>
+          <t>claudia lin</t>
         </is>
       </c>
       <c r="N5" s="6" t="inlineStr">
@@ -758,49 +758,49 @@
       </c>
       <c r="O5" s="9" t="inlineStr">
         <is>
-          <t>Rachel Kim</t>
+          <t>Jiwang Lee</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="C6" s="1" t="inlineStr">
         <is>
+          <t>Aaron Long</t>
+        </is>
+      </c>
+      <c r="D6" s="1" t="inlineStr">
+        <is>
+          <t>JJ Lee</t>
+        </is>
+      </c>
+      <c r="E6" s="9" t="inlineStr">
+        <is>
+          <t>Joann Jung</t>
+        </is>
+      </c>
+      <c r="F6" s="9" t="inlineStr">
+        <is>
+          <t>Jeffery Huang</t>
+        </is>
+      </c>
+      <c r="G6" s="6" t="inlineStr">
+        <is>
+          <t>Samuel Wen</t>
+        </is>
+      </c>
+      <c r="K6" s="1" t="inlineStr">
+        <is>
           <t>Nathanael Wang</t>
         </is>
       </c>
-      <c r="D6" s="1" t="inlineStr">
-        <is>
-          <t>Phillip Seo</t>
-        </is>
-      </c>
-      <c r="E6" s="9" t="inlineStr">
-        <is>
-          <t>Jeffery Huang</t>
-        </is>
-      </c>
-      <c r="F6" s="9" t="inlineStr">
-        <is>
-          <t>Daniel Kuo</t>
-        </is>
-      </c>
-      <c r="G6" s="6" t="inlineStr">
+      <c r="L6" s="6" t="inlineStr">
         <is>
           <t>Logan Golia</t>
         </is>
       </c>
-      <c r="K6" s="1" t="inlineStr">
-        <is>
-          <t>Christina Ko</t>
-        </is>
-      </c>
-      <c r="L6" s="6" t="inlineStr">
-        <is>
-          <t>Samuel Wen</t>
-        </is>
-      </c>
       <c r="M6" s="9" t="inlineStr">
         <is>
-          <t>Grace Kwon</t>
+          <t xml:space="preserve">Derek Liang </t>
         </is>
       </c>
       <c r="N6" s="7" t="inlineStr">
@@ -810,7 +810,7 @@
       </c>
       <c r="O6" s="9" t="inlineStr">
         <is>
-          <t>Claire Doh</t>
+          <t>Israel Haile</t>
         </is>
       </c>
     </row>
@@ -881,27 +881,27 @@
       </c>
       <c r="E10" s="9" t="inlineStr">
         <is>
-          <t>Grace Kwon</t>
+          <t>Jiwang Lee</t>
         </is>
       </c>
       <c r="F10" s="6" t="inlineStr">
         <is>
-          <t>Daniel Song</t>
+          <t>Justin Zhang</t>
         </is>
       </c>
       <c r="G10" s="6" t="inlineStr">
         <is>
-          <t>Sabrina Sun</t>
+          <t>Logan Golia</t>
         </is>
       </c>
       <c r="K10" s="9" t="inlineStr">
         <is>
-          <t xml:space="preserve">Derek Liang </t>
+          <t>Hannah Kim</t>
         </is>
       </c>
       <c r="L10" s="9" t="inlineStr">
         <is>
-          <t>Daniel Kuo</t>
+          <t>Rachel Kim</t>
         </is>
       </c>
       <c r="M10" s="7" t="inlineStr">
@@ -928,17 +928,17 @@
       </c>
       <c r="E11" s="9" t="inlineStr">
         <is>
-          <t xml:space="preserve">Derek Liang </t>
+          <t>Benjamin Kim</t>
         </is>
       </c>
       <c r="F11" s="6" t="inlineStr">
         <is>
-          <t>Justin Zhang</t>
+          <t xml:space="preserve">Daniel Kim </t>
         </is>
       </c>
       <c r="G11" s="6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Daniel Kim </t>
+          <t>Jocelyn Youn</t>
         </is>
       </c>
       <c r="K11" s="9" t="inlineStr">
@@ -948,12 +948,12 @@
       </c>
       <c r="L11" s="9" t="inlineStr">
         <is>
-          <t>Joann Jung</t>
+          <t>Claire Doh</t>
         </is>
       </c>
       <c r="N11" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">Michael Dong </t>
+          <t>Aaron Long</t>
         </is>
       </c>
       <c r="O11" s="6" t="inlineStr">
@@ -970,32 +970,32 @@
       </c>
       <c r="E12" s="9" t="inlineStr">
         <is>
+          <t>Grace Kwon</t>
+        </is>
+      </c>
+      <c r="F12" s="6" t="inlineStr">
+        <is>
+          <t>Daniel Song</t>
+        </is>
+      </c>
+      <c r="G12" s="7" t="inlineStr">
+        <is>
+          <t>Jeff Jiang</t>
+        </is>
+      </c>
+      <c r="K12" s="9" t="inlineStr">
+        <is>
+          <t>David Zhu</t>
+        </is>
+      </c>
+      <c r="L12" s="9" t="inlineStr">
+        <is>
           <t>Joann Jung</t>
         </is>
       </c>
-      <c r="F12" s="6" t="inlineStr">
-        <is>
-          <t>Samuel Wen</t>
-        </is>
-      </c>
-      <c r="G12" s="7" t="inlineStr">
-        <is>
-          <t>Sam Ko</t>
-        </is>
-      </c>
-      <c r="K12" s="9" t="inlineStr">
-        <is>
-          <t>Hannah Kim</t>
-        </is>
-      </c>
-      <c r="L12" s="9" t="inlineStr">
-        <is>
-          <t>Jiwang Lee</t>
-        </is>
-      </c>
       <c r="N12" s="1" t="inlineStr">
         <is>
-          <t>Aaron Long</t>
+          <t xml:space="preserve">Michael Dong </t>
         </is>
       </c>
       <c r="O12" s="9" t="inlineStr">
@@ -1012,27 +1012,27 @@
       </c>
       <c r="E13" s="9" t="inlineStr">
         <is>
-          <t>Benjamin Kim</t>
+          <t>Claire Doh</t>
         </is>
       </c>
       <c r="F13" s="9" t="inlineStr">
         <is>
-          <t>Kyle Hwang</t>
+          <t>Hannah Kim</t>
         </is>
       </c>
       <c r="G13" s="7" t="inlineStr">
         <is>
-          <t>Jeff Jiang</t>
+          <t>Sam Ko</t>
         </is>
       </c>
       <c r="K13" s="9" t="inlineStr">
         <is>
-          <t>David Zhu</t>
+          <t>Grace Kwon</t>
         </is>
       </c>
       <c r="L13" s="9" t="inlineStr">
         <is>
-          <t>Israel Haile</t>
+          <t>Daniel Kuo</t>
         </is>
       </c>
       <c r="N13" s="7" t="inlineStr">
@@ -1068,7 +1068,7 @@
     <row r="17">
       <c r="C17" s="9" t="inlineStr">
         <is>
-          <t>Jiwang Lee</t>
+          <t xml:space="preserve">Derek Liang </t>
         </is>
       </c>
       <c r="D17" s="9" t="inlineStr">
@@ -1090,7 +1090,7 @@
     <row r="18">
       <c r="C18" s="9" t="inlineStr">
         <is>
-          <t>Israel Haile</t>
+          <t>Taeho Choe</t>
         </is>
       </c>
       <c r="K18" s="7" t="inlineStr">
@@ -1107,7 +1107,7 @@
     <row r="19">
       <c r="C19" s="9" t="inlineStr">
         <is>
-          <t>Taeho Choe</t>
+          <t>David Zhu</t>
         </is>
       </c>
       <c r="K19" s="9" t="inlineStr">
@@ -1119,7 +1119,7 @@
     <row r="20">
       <c r="C20" s="9" t="inlineStr">
         <is>
-          <t>Hannah Kim</t>
+          <t>Israel Haile</t>
         </is>
       </c>
       <c r="K20" s="9" t="inlineStr">

</xml_diff>

<commit_message>
use folium to improve interactive map of assignments
</commit_message>
<xml_diff>
--- a/api_allocate.xlsx
+++ b/api_allocate.xlsx
@@ -30,7 +30,7 @@
       <u val="single"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill/>
     </fill>
@@ -57,6 +57,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFd9ead3"/>
+        <bgColor rgb="FFd9ead3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFCCCCCC"/>
         <bgColor rgb="FFCCCCCC"/>
       </patternFill>
@@ -69,14 +75,20 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFCFE2F3"/>
+        <bgColor rgb="FFCFE2F3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFCE5CD"/>
         <bgColor rgb="FFFCE5CD"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FFFFFF"/>
-        <bgColor rgb="00FFFFFF"/>
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FFD9D9D9"/>
       </patternFill>
     </fill>
   </fills>
@@ -92,32 +104,43 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -483,7 +506,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:P6"/>
+  <dimension ref="B1:O24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -492,17 +515,17 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="6" customWidth="1" min="2" max="2"/>
-    <col width="20" customWidth="1" min="3" max="3"/>
-    <col width="19" customWidth="1" min="4" max="4"/>
+    <col width="21" customWidth="1" min="3" max="3"/>
+    <col width="42" customWidth="1" min="4" max="4"/>
     <col width="20" customWidth="1" min="5" max="5"/>
-    <col width="20" customWidth="1" min="6" max="6"/>
-    <col width="42" customWidth="1" min="8" max="8"/>
+    <col width="22" customWidth="1" min="6" max="6"/>
+    <col width="19" customWidth="1" min="7" max="7"/>
     <col width="12" customWidth="1" min="10" max="10"/>
-    <col width="20" customWidth="1" min="11" max="11"/>
-    <col width="19" customWidth="1" min="12" max="12"/>
+    <col width="21" customWidth="1" min="11" max="11"/>
+    <col width="21" customWidth="1" min="12" max="12"/>
     <col width="20" customWidth="1" min="13" max="13"/>
-    <col width="20" customWidth="1" min="14" max="14"/>
-    <col width="68" customWidth="1" min="16" max="16"/>
+    <col width="22" customWidth="1" min="14" max="14"/>
+    <col width="70" customWidth="1" min="15" max="15"/>
   </cols>
   <sheetData>
     <row r="1"/>
@@ -514,235 +537,687 @@
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
+          <t>Driver: Olivia Chang</t>
+        </is>
+      </c>
+      <c r="D2" s="2" t="inlineStr">
+        <is>
+          <t>Driver: Clay Murphy</t>
+        </is>
+      </c>
+      <c r="E2" s="2" t="inlineStr">
+        <is>
           <t>Driver: Matthew Ahn</t>
         </is>
       </c>
-      <c r="D2" s="2" t="inlineStr">
-        <is>
-          <t>Driver: Aaron Long</t>
-        </is>
-      </c>
-      <c r="E2" s="2" t="inlineStr">
+      <c r="F2" s="2" t="inlineStr">
+        <is>
+          <t>Driver: Jack Havemann</t>
+        </is>
+      </c>
+      <c r="G2" s="3" t="inlineStr">
+        <is>
+          <t>Driver: Jenny Sohn</t>
+        </is>
+      </c>
+      <c r="J2" s="4" t="inlineStr">
+        <is>
+          <t>Back home 💙</t>
+        </is>
+      </c>
+      <c r="K2" s="5" t="inlineStr">
+        <is>
+          <t>Driver: Olivia Chang</t>
+        </is>
+      </c>
+      <c r="L2" s="5" t="inlineStr">
+        <is>
+          <t>Driver: Matthew Ahn</t>
+        </is>
+      </c>
+      <c r="M2" s="5" t="inlineStr">
+        <is>
+          <t>Driver: Jenny Sohn</t>
+        </is>
+      </c>
+      <c r="N2" s="5" t="inlineStr">
+        <is>
+          <t>Driver: Jocelyn Lee</t>
+        </is>
+      </c>
+      <c r="O2" s="5" t="inlineStr">
+        <is>
+          <t>Driver: Rebecca Lu</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" s="6" t="inlineStr">
+        <is>
+          <t>North</t>
+        </is>
+      </c>
+      <c r="C3" s="7" t="inlineStr">
+        <is>
+          <t>Shayla Nguyen</t>
+        </is>
+      </c>
+      <c r="D3" s="1" t="inlineStr">
+        <is>
+          <t>JJ Lee</t>
+        </is>
+      </c>
+      <c r="E3" s="1" t="inlineStr">
+        <is>
+          <t>Melody Hong</t>
+        </is>
+      </c>
+      <c r="F3" s="7" t="inlineStr">
+        <is>
+          <t>Faith Chen</t>
+        </is>
+      </c>
+      <c r="G3" s="6" t="inlineStr">
+        <is>
+          <t>Emily Yang</t>
+        </is>
+      </c>
+      <c r="J3" s="8" t="inlineStr">
+        <is>
+          <t>Flexible 💚</t>
+        </is>
+      </c>
+      <c r="K3" s="1" t="inlineStr">
+        <is>
+          <t>Christina Ko</t>
+        </is>
+      </c>
+      <c r="L3" s="9" t="inlineStr">
+        <is>
+          <t>Aaron duong</t>
+        </is>
+      </c>
+      <c r="M3" s="9" t="inlineStr">
+        <is>
+          <t>Jiwang Lee</t>
+        </is>
+      </c>
+      <c r="N3" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">derek liang </t>
+        </is>
+      </c>
+      <c r="O3" s="6" t="inlineStr">
+        <is>
+          <t>Lucy Han</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" s="7" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="C4" s="7" t="inlineStr">
+        <is>
+          <t>Pedro Flores-Teran</t>
+        </is>
+      </c>
+      <c r="D4" s="1" t="inlineStr">
+        <is>
+          <t>Nathanael Wang</t>
+        </is>
+      </c>
+      <c r="E4" s="1" t="inlineStr">
+        <is>
+          <t>Ethan Yu</t>
+        </is>
+      </c>
+      <c r="F4" s="9" t="inlineStr">
+        <is>
+          <t>Taeho Choe</t>
+        </is>
+      </c>
+      <c r="G4" s="6" t="inlineStr">
+        <is>
+          <t>Gabriel Ni</t>
+        </is>
+      </c>
+      <c r="J4" s="10" t="inlineStr">
+        <is>
+          <t>Lunch 💛</t>
+        </is>
+      </c>
+      <c r="K4" s="1" t="inlineStr">
+        <is>
+          <t>Sehyun Jung</t>
+        </is>
+      </c>
+      <c r="L4" s="9" t="inlineStr">
+        <is>
+          <t>Israel Haile</t>
+        </is>
+      </c>
+      <c r="M4" s="9" t="inlineStr">
+        <is>
+          <t>Hannah Kim</t>
+        </is>
+      </c>
+      <c r="N4" s="9" t="inlineStr">
+        <is>
+          <t>Rachel Kim</t>
+        </is>
+      </c>
+      <c r="O4" s="6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Darius Ajebon </t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" s="9" t="inlineStr">
+        <is>
+          <t>South</t>
+        </is>
+      </c>
+      <c r="D5" s="1" t="inlineStr">
+        <is>
+          <t>Grace Park</t>
+        </is>
+      </c>
+      <c r="E5" s="1" t="inlineStr">
+        <is>
+          <t>Sehyun Jung</t>
+        </is>
+      </c>
+      <c r="F5" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Maya Habraken </t>
+        </is>
+      </c>
+      <c r="G5" s="9" t="inlineStr">
+        <is>
+          <t>Grace Kwon</t>
+        </is>
+      </c>
+      <c r="J5" s="11" t="inlineStr">
+        <is>
+          <t>NLK 🧡</t>
+        </is>
+      </c>
+      <c r="K5" s="1" t="inlineStr">
+        <is>
+          <t>Nathanael Wang</t>
+        </is>
+      </c>
+      <c r="L5" s="7" t="inlineStr">
+        <is>
+          <t>Jane Yoo</t>
+        </is>
+      </c>
+      <c r="M5" s="9" t="inlineStr">
+        <is>
+          <t>Taeho Choe</t>
+        </is>
+      </c>
+      <c r="N5" s="9" t="inlineStr">
+        <is>
+          <t>Daniel Kuo</t>
+        </is>
+      </c>
+      <c r="O5" s="6" t="inlineStr">
+        <is>
+          <t>Daniel Song</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="D6" s="1" t="inlineStr">
+        <is>
+          <t>Christina Ko</t>
+        </is>
+      </c>
+      <c r="E6" s="1" t="inlineStr">
+        <is>
+          <t>Joanna Wei</t>
+        </is>
+      </c>
+      <c r="F6" s="9" t="inlineStr">
+        <is>
+          <t>Hannah Kim</t>
+        </is>
+      </c>
+      <c r="G6" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">derek liang </t>
+        </is>
+      </c>
+      <c r="K6" s="1" t="inlineStr">
+        <is>
+          <t>Grace Park</t>
+        </is>
+      </c>
+      <c r="L6" s="6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Daniel Kim </t>
+        </is>
+      </c>
+      <c r="M6" s="9" t="inlineStr">
+        <is>
+          <t>Kyle Hwang</t>
+        </is>
+      </c>
+      <c r="N6" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Grace Sowon Park </t>
+        </is>
+      </c>
+      <c r="O6" s="6" t="inlineStr">
+        <is>
+          <t>Emily Yang</t>
+        </is>
+      </c>
+    </row>
+    <row r="7"/>
+    <row r="8"/>
+    <row r="9">
+      <c r="C9" s="3" t="inlineStr">
+        <is>
+          <t>Driver: Jonathan Mak</t>
+        </is>
+      </c>
+      <c r="D9" s="12" t="inlineStr">
+        <is>
+          <t>Driver: Jocelyn Lee</t>
+        </is>
+      </c>
+      <c r="E9" s="12" t="inlineStr">
+        <is>
+          <t>Driver: Rebecca Lu</t>
+        </is>
+      </c>
+      <c r="F9" s="12" t="inlineStr">
+        <is>
+          <t>Driver: Daniel Choi</t>
+        </is>
+      </c>
+      <c r="G9" s="12" t="inlineStr">
+        <is>
+          <t>Driver: Josh Paik</t>
+        </is>
+      </c>
+      <c r="K9" s="13" t="inlineStr">
         <is>
           <t>Driver: Clay Murphy</t>
         </is>
       </c>
-      <c r="F2" s="3" t="inlineStr">
+      <c r="L9" s="13" t="inlineStr">
+        <is>
+          <t>Driver: david kim</t>
+        </is>
+      </c>
+      <c r="M9" s="13" t="inlineStr">
+        <is>
+          <t>Driver: Ric Chang</t>
+        </is>
+      </c>
+      <c r="N9" s="14" t="inlineStr">
+        <is>
+          <t>Driver: Jack Havemann</t>
+        </is>
+      </c>
+      <c r="O9" s="14" t="inlineStr">
+        <is>
+          <t>Driver: Daniel Choi</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="C10" s="6" t="inlineStr">
+        <is>
+          <t>Lucy Han</t>
+        </is>
+      </c>
+      <c r="D10" s="7" t="inlineStr">
+        <is>
+          <t>Seojin Kwon</t>
+        </is>
+      </c>
+      <c r="E10" s="7" t="inlineStr">
+        <is>
+          <t>Kaitlyn Kim</t>
+        </is>
+      </c>
+      <c r="F10" s="7" t="inlineStr">
+        <is>
+          <t>Jane Yoo</t>
+        </is>
+      </c>
+      <c r="G10" s="7" t="inlineStr">
+        <is>
+          <t>Austin Lee</t>
+        </is>
+      </c>
+      <c r="K10" s="9" t="inlineStr">
+        <is>
+          <t>Ella Lu</t>
+        </is>
+      </c>
+      <c r="L10" s="7" t="inlineStr">
+        <is>
+          <t>Seojin Kwon</t>
+        </is>
+      </c>
+      <c r="M10" s="9" t="inlineStr">
+        <is>
+          <t>Elie Park</t>
+        </is>
+      </c>
+      <c r="N10" s="1" t="inlineStr">
+        <is>
+          <t>JJ Lee</t>
+        </is>
+      </c>
+      <c r="O10" s="7" t="inlineStr">
+        <is>
+          <t>Khang Le</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="C11" s="6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Darius Ajebon </t>
+        </is>
+      </c>
+      <c r="E11" s="7" t="inlineStr">
+        <is>
+          <t>Khang Le</t>
+        </is>
+      </c>
+      <c r="F11" s="9" t="inlineStr">
+        <is>
+          <t>Joann Jung</t>
+        </is>
+      </c>
+      <c r="G11" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Grace Sowon Park </t>
+        </is>
+      </c>
+      <c r="K11" s="9" t="inlineStr">
+        <is>
+          <t>Hyeongjun Son</t>
+        </is>
+      </c>
+      <c r="L11" s="7" t="inlineStr">
+        <is>
+          <t>Sam Ko</t>
+        </is>
+      </c>
+      <c r="M11" s="9" t="inlineStr">
+        <is>
+          <t>Joann Jung</t>
+        </is>
+      </c>
+      <c r="N11" s="1" t="inlineStr">
+        <is>
+          <t>Ethan Yu</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="C12" s="6" t="inlineStr">
+        <is>
+          <t>Daniel Song</t>
+        </is>
+      </c>
+      <c r="F12" s="9" t="inlineStr">
+        <is>
+          <t>Jiwang Lee</t>
+        </is>
+      </c>
+      <c r="G12" s="9" t="inlineStr">
+        <is>
+          <t>Daniel Kuo</t>
+        </is>
+      </c>
+      <c r="K12" s="7" t="inlineStr">
+        <is>
+          <t>Shayla Nguyen</t>
+        </is>
+      </c>
+      <c r="L12" s="6" t="inlineStr">
+        <is>
+          <t>Jocelyn Youn</t>
+        </is>
+      </c>
+      <c r="M12" s="7" t="inlineStr">
+        <is>
+          <t>April Tong</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="C13" s="6" t="inlineStr">
+        <is>
+          <t>Jocelyn Youn</t>
+        </is>
+      </c>
+      <c r="F13" s="9" t="inlineStr">
+        <is>
+          <t>Rachel Kim</t>
+        </is>
+      </c>
+      <c r="G13" s="9" t="inlineStr">
+        <is>
+          <t>Ella Lu</t>
+        </is>
+      </c>
+      <c r="K13" s="7" t="inlineStr">
+        <is>
+          <t>Pedro Flores-Teran</t>
+        </is>
+      </c>
+      <c r="M13" s="6" t="inlineStr">
+        <is>
+          <t>Gabriel Ni</t>
+        </is>
+      </c>
+    </row>
+    <row r="14"/>
+    <row r="15"/>
+    <row r="16">
+      <c r="C16" s="12" t="inlineStr">
+        <is>
+          <t>Driver: david kim</t>
+        </is>
+      </c>
+      <c r="D16" s="12" t="inlineStr">
+        <is>
+          <t>Driver: Lia kim</t>
+        </is>
+      </c>
+      <c r="E16" s="12" t="inlineStr">
+        <is>
+          <t>Driver: Ric Chang</t>
+        </is>
+      </c>
+      <c r="F16" s="15" t="inlineStr">
+        <is>
+          <t>Driver: Brian Seo</t>
+        </is>
+      </c>
+      <c r="G16" s="15" t="inlineStr">
+        <is>
+          <t>Driver: AZ Ellis</t>
+        </is>
+      </c>
+      <c r="K16" s="14" t="inlineStr">
+        <is>
+          <t>Driver: Brian Seo</t>
+        </is>
+      </c>
+      <c r="L16" s="14" t="inlineStr">
+        <is>
+          <t>Driver: Jonathan Mak</t>
+        </is>
+      </c>
+      <c r="M16" s="16" t="inlineStr">
         <is>
           <t>Driver: Oriana Tang</t>
         </is>
       </c>
-      <c r="H2" s="4" t="inlineStr">
+      <c r="O16" s="17" t="inlineStr">
         <is>
           <t>UNASSIGNED RIDERS</t>
         </is>
       </c>
-      <c r="J2" s="5" t="inlineStr">
-        <is>
-          <t>Back home 💙</t>
-        </is>
-      </c>
-      <c r="K2" s="6" t="inlineStr">
-        <is>
-          <t>Driver: Clay Murphy</t>
-        </is>
-      </c>
-      <c r="L2" s="7" t="inlineStr">
-        <is>
-          <t>Driver: Aaron Long</t>
-        </is>
-      </c>
-      <c r="M2" s="7" t="inlineStr">
-        <is>
-          <t>Driver: Matthew Ahn</t>
-        </is>
-      </c>
-      <c r="N2" s="8" t="inlineStr">
-        <is>
-          <t>Driver: Oriana Tang</t>
-        </is>
-      </c>
-      <c r="P2" s="4" t="inlineStr">
+    </row>
+    <row r="17">
+      <c r="C17" s="7" t="inlineStr">
+        <is>
+          <t>April Tong</t>
+        </is>
+      </c>
+      <c r="D17" s="6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Daniel Kim </t>
+        </is>
+      </c>
+      <c r="E17" s="7" t="inlineStr">
+        <is>
+          <t>Sam Ko</t>
+        </is>
+      </c>
+      <c r="F17" s="9" t="inlineStr">
+        <is>
+          <t>Israel Haile</t>
+        </is>
+      </c>
+      <c r="G17" s="9" t="inlineStr">
+        <is>
+          <t>Kyle Hwang</t>
+        </is>
+      </c>
+      <c r="K17" s="9" t="inlineStr">
+        <is>
+          <t>Benjamin Kim</t>
+        </is>
+      </c>
+      <c r="L17" s="6" t="inlineStr">
+        <is>
+          <t>helena song</t>
+        </is>
+      </c>
+      <c r="M17" s="1" t="inlineStr">
+        <is>
+          <t>Melody Hong</t>
+        </is>
+      </c>
+      <c r="O17" s="1" t="inlineStr">
+        <is>
+          <t>Joanna Wei (RJM 🩵) No valid driver available to assign this driver</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="D18" s="6" t="inlineStr">
+        <is>
+          <t>helena song</t>
+        </is>
+      </c>
+      <c r="F18" s="9" t="inlineStr">
+        <is>
+          <t>Hannah Zhang</t>
+        </is>
+      </c>
+      <c r="G18" s="9" t="inlineStr">
+        <is>
+          <t>Benjamin Kim</t>
+        </is>
+      </c>
+      <c r="K18" s="9" t="inlineStr">
+        <is>
+          <t>Hannah Zhang</t>
+        </is>
+      </c>
+      <c r="O18" s="7" t="inlineStr">
+        <is>
+          <t>Kaitlyn Kim (RJM 🩵) No valid driver available to assign this driver</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="F19" s="9" t="inlineStr">
+        <is>
+          <t>Aaron duong</t>
+        </is>
+      </c>
+      <c r="G19" s="9" t="inlineStr">
+        <is>
+          <t>Hyeongjun Son</t>
+        </is>
+      </c>
+      <c r="K19" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Maya Habraken </t>
+        </is>
+      </c>
+      <c r="O19" s="7" t="inlineStr">
+        <is>
+          <t>Bless Hwang  (Lunch 💛) (invalid off campus address)</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="F20" s="9" t="inlineStr">
+        <is>
+          <t>Jeffery Huang</t>
+        </is>
+      </c>
+      <c r="G20" s="9" t="inlineStr">
+        <is>
+          <t>Elie Park</t>
+        </is>
+      </c>
+      <c r="K20" s="9" t="inlineStr">
+        <is>
+          <t>Grace Kwon</t>
+        </is>
+      </c>
+      <c r="O20" s="7" t="inlineStr">
+        <is>
+          <t>Austin Lee (RJM 🩵) No valid driver available to assign this driver</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="O21" s="7" t="inlineStr">
+        <is>
+          <t>Faith Chen (RJM 🩵) No valid driver available to assign this driver</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="O22" s="9" t="inlineStr">
+        <is>
+          <t>Jeffery Huang (RJM 🩵) No valid driver available to assign this driver</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="D23" s="17" t="inlineStr">
         <is>
           <t>UNASSIGNED RIDERS</t>
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="B3" s="9" t="inlineStr">
-        <is>
-          <t>Off</t>
-        </is>
-      </c>
-      <c r="C3" s="9" t="inlineStr">
-        <is>
-          <t>david kim</t>
-        </is>
-      </c>
-      <c r="D3" s="1" t="inlineStr">
-        <is>
-          <t>Grace Park</t>
-        </is>
-      </c>
-      <c r="E3" s="9" t="inlineStr">
-        <is>
-          <t>Faith Chen</t>
-        </is>
-      </c>
-      <c r="F3" s="9" t="inlineStr">
-        <is>
-          <t>Sam Ko</t>
-        </is>
-      </c>
-      <c r="H3" s="9" t="inlineStr">
+    <row r="24">
+      <c r="D24" s="7" t="inlineStr">
         <is>
           <t>Bless Hwang  (invalid off campus address)</t>
-        </is>
-      </c>
-      <c r="J3" s="10" t="inlineStr">
-        <is>
-          <t>Lunch 💛</t>
-        </is>
-      </c>
-      <c r="K3" s="1" t="inlineStr">
-        <is>
-          <t>Grace Park</t>
-        </is>
-      </c>
-      <c r="L3" s="9" t="inlineStr">
-        <is>
-          <t>david kim</t>
-        </is>
-      </c>
-      <c r="M3" s="1" t="inlineStr">
-        <is>
-          <t>Ethan Yu</t>
-        </is>
-      </c>
-      <c r="N3" s="11" t="inlineStr">
-        <is>
-          <t>derek liang</t>
-        </is>
-      </c>
-      <c r="P3" s="9" t="inlineStr">
-        <is>
-          <t>Bless Hwang  (NLK 🧡) (invalid off campus address)</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="B4" s="11" t="inlineStr">
-        <is>
-          <t>South</t>
-        </is>
-      </c>
-      <c r="C4" s="9" t="inlineStr">
-        <is>
-          <t>Seojin Kwon</t>
-        </is>
-      </c>
-      <c r="D4" s="1" t="inlineStr">
-        <is>
-          <t>Jocelyn Youn</t>
-        </is>
-      </c>
-      <c r="E4" s="11" t="inlineStr">
-        <is>
-          <t>derek liang</t>
-        </is>
-      </c>
-      <c r="F4" s="9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Benjamin Kim </t>
-        </is>
-      </c>
-      <c r="J4" s="12" t="inlineStr">
-        <is>
-          <t>TLBS Grad 🩵</t>
-        </is>
-      </c>
-      <c r="K4" s="1" t="inlineStr">
-        <is>
-          <t>Melody Hong</t>
-        </is>
-      </c>
-      <c r="L4" s="9" t="inlineStr">
-        <is>
-          <t>Seojin Kwon</t>
-        </is>
-      </c>
-      <c r="M4" s="1" t="inlineStr">
-        <is>
-          <t>Jocelyn Youn</t>
-        </is>
-      </c>
-      <c r="P4" s="11" t="inlineStr">
-        <is>
-          <t>David zhu (Lunch 💛) No valid driver available to assign this driver</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="C5" s="9" t="inlineStr">
-        <is>
-          <t>Stella Son</t>
-        </is>
-      </c>
-      <c r="D5" s="1" t="inlineStr">
-        <is>
-          <t>Ethan Yu</t>
-        </is>
-      </c>
-      <c r="E5" s="11" t="inlineStr">
-        <is>
-          <t>David zhu</t>
-        </is>
-      </c>
-      <c r="K5" s="9" t="inlineStr">
-        <is>
-          <t>Stella Son</t>
-        </is>
-      </c>
-      <c r="L5" s="9" t="inlineStr">
-        <is>
-          <t>Sam Ko</t>
-        </is>
-      </c>
-      <c r="M5" s="9" t="inlineStr">
-        <is>
-          <t>Faith Chen</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="C6" s="9" t="inlineStr">
-        <is>
-          <t>Khang Le</t>
-        </is>
-      </c>
-      <c r="D6" s="1" t="inlineStr">
-        <is>
-          <t>Melody Hong</t>
-        </is>
-      </c>
-      <c r="E6" s="11" t="inlineStr">
-        <is>
-          <t>Kyle Hwang</t>
-        </is>
-      </c>
-      <c r="K6" s="11" t="inlineStr">
-        <is>
-          <t>Kyle Hwang</t>
-        </is>
-      </c>
-      <c r="L6" s="9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Benjamin Kim </t>
-        </is>
-      </c>
-      <c r="M6" s="9" t="inlineStr">
-        <is>
-          <t>Khang Le</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
clean file structure for deployment to gh pages
</commit_message>
<xml_diff>
--- a/api_allocate.xlsx
+++ b/api_allocate.xlsx
@@ -515,13 +515,13 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="6" customWidth="1" min="2" max="2"/>
-    <col width="21" customWidth="1" min="3" max="3"/>
+    <col width="22" customWidth="1" min="3" max="3"/>
     <col width="42" customWidth="1" min="4" max="4"/>
     <col width="20" customWidth="1" min="5" max="5"/>
-    <col width="22" customWidth="1" min="6" max="6"/>
-    <col width="19" customWidth="1" min="7" max="7"/>
+    <col width="21" customWidth="1" min="6" max="6"/>
+    <col width="21" customWidth="1" min="7" max="7"/>
     <col width="12" customWidth="1" min="10" max="10"/>
-    <col width="21" customWidth="1" min="11" max="11"/>
+    <col width="20" customWidth="1" min="11" max="11"/>
     <col width="21" customWidth="1" min="12" max="12"/>
     <col width="20" customWidth="1" min="13" max="13"/>
     <col width="22" customWidth="1" min="14" max="14"/>
@@ -537,42 +537,42 @@
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
+          <t>Driver: Jack Havemann</t>
+        </is>
+      </c>
+      <c r="D2" s="2" t="inlineStr">
+        <is>
+          <t>Driver: Clay Murphy</t>
+        </is>
+      </c>
+      <c r="E2" s="2" t="inlineStr">
+        <is>
+          <t>Driver: Matthew Ahn</t>
+        </is>
+      </c>
+      <c r="F2" s="2" t="inlineStr">
+        <is>
           <t>Driver: Olivia Chang</t>
         </is>
       </c>
-      <c r="D2" s="2" t="inlineStr">
-        <is>
-          <t>Driver: Clay Murphy</t>
-        </is>
-      </c>
-      <c r="E2" s="2" t="inlineStr">
+      <c r="G2" s="3" t="inlineStr">
+        <is>
+          <t>Driver: Jonathan Mak</t>
+        </is>
+      </c>
+      <c r="J2" s="4" t="inlineStr">
+        <is>
+          <t>Back home 💙</t>
+        </is>
+      </c>
+      <c r="K2" s="5" t="inlineStr">
         <is>
           <t>Driver: Matthew Ahn</t>
         </is>
       </c>
-      <c r="F2" s="2" t="inlineStr">
-        <is>
-          <t>Driver: Jack Havemann</t>
-        </is>
-      </c>
-      <c r="G2" s="3" t="inlineStr">
-        <is>
-          <t>Driver: Jenny Sohn</t>
-        </is>
-      </c>
-      <c r="J2" s="4" t="inlineStr">
-        <is>
-          <t>Back home 💙</t>
-        </is>
-      </c>
-      <c r="K2" s="5" t="inlineStr">
+      <c r="L2" s="5" t="inlineStr">
         <is>
           <t>Driver: Olivia Chang</t>
-        </is>
-      </c>
-      <c r="L2" s="5" t="inlineStr">
-        <is>
-          <t>Driver: Matthew Ahn</t>
         </is>
       </c>
       <c r="M2" s="5" t="inlineStr">
@@ -599,17 +599,17 @@
       </c>
       <c r="C3" s="7" t="inlineStr">
         <is>
-          <t>Shayla Nguyen</t>
+          <t>Pedro Flores-Teran</t>
         </is>
       </c>
       <c r="D3" s="1" t="inlineStr">
         <is>
-          <t>JJ Lee</t>
+          <t>Sehyun Jung</t>
         </is>
       </c>
       <c r="E3" s="1" t="inlineStr">
         <is>
-          <t>Melody Hong</t>
+          <t>Nathanael Wang</t>
         </is>
       </c>
       <c r="F3" s="7" t="inlineStr">
@@ -619,7 +619,7 @@
       </c>
       <c r="G3" s="6" t="inlineStr">
         <is>
-          <t>Emily Yang</t>
+          <t>Daniel Song</t>
         </is>
       </c>
       <c r="J3" s="8" t="inlineStr">
@@ -629,19 +629,19 @@
       </c>
       <c r="K3" s="1" t="inlineStr">
         <is>
-          <t>Christina Ko</t>
-        </is>
-      </c>
-      <c r="L3" s="9" t="inlineStr">
+          <t>Sehyun Jung</t>
+        </is>
+      </c>
+      <c r="L3" s="6" t="inlineStr">
+        <is>
+          <t>Lucy Han</t>
+        </is>
+      </c>
+      <c r="M3" s="9" t="inlineStr">
         <is>
           <t>Aaron duong</t>
         </is>
       </c>
-      <c r="M3" s="9" t="inlineStr">
-        <is>
-          <t>Jiwang Lee</t>
-        </is>
-      </c>
       <c r="N3" s="9" t="inlineStr">
         <is>
           <t xml:space="preserve">derek liang </t>
@@ -649,7 +649,7 @@
       </c>
       <c r="O3" s="6" t="inlineStr">
         <is>
-          <t>Lucy Han</t>
+          <t xml:space="preserve">Darius Ajebon </t>
         </is>
       </c>
     </row>
@@ -661,27 +661,27 @@
       </c>
       <c r="C4" s="7" t="inlineStr">
         <is>
-          <t>Pedro Flores-Teran</t>
+          <t>Shayla Nguyen</t>
         </is>
       </c>
       <c r="D4" s="1" t="inlineStr">
         <is>
-          <t>Nathanael Wang</t>
+          <t>JJ Lee</t>
         </is>
       </c>
       <c r="E4" s="1" t="inlineStr">
         <is>
-          <t>Ethan Yu</t>
+          <t>Grace Park</t>
         </is>
       </c>
       <c r="F4" s="9" t="inlineStr">
         <is>
-          <t>Taeho Choe</t>
+          <t>Jiwang Lee</t>
         </is>
       </c>
       <c r="G4" s="6" t="inlineStr">
         <is>
-          <t>Gabriel Ni</t>
+          <t>Jocelyn Youn</t>
         </is>
       </c>
       <c r="J4" s="10" t="inlineStr">
@@ -691,12 +691,12 @@
       </c>
       <c r="K4" s="1" t="inlineStr">
         <is>
-          <t>Sehyun Jung</t>
-        </is>
-      </c>
-      <c r="L4" s="9" t="inlineStr">
-        <is>
-          <t>Israel Haile</t>
+          <t>Christina Ko</t>
+        </is>
+      </c>
+      <c r="L4" s="7" t="inlineStr">
+        <is>
+          <t>Jane Yoo</t>
         </is>
       </c>
       <c r="M4" s="9" t="inlineStr">
@@ -706,12 +706,12 @@
       </c>
       <c r="N4" s="9" t="inlineStr">
         <is>
-          <t>Rachel Kim</t>
+          <t>Jiwang Lee</t>
         </is>
       </c>
       <c r="O4" s="6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Darius Ajebon </t>
+          <t xml:space="preserve">Daniel Kim </t>
         </is>
       </c>
     </row>
@@ -723,22 +723,22 @@
       </c>
       <c r="D5" s="1" t="inlineStr">
         <is>
-          <t>Grace Park</t>
+          <t>Christina Ko</t>
         </is>
       </c>
       <c r="E5" s="1" t="inlineStr">
         <is>
-          <t>Sehyun Jung</t>
+          <t>Ethan Yu</t>
         </is>
       </c>
       <c r="F5" s="9" t="inlineStr">
         <is>
-          <t xml:space="preserve">Maya Habraken </t>
+          <t>Hyeongjun Son</t>
         </is>
       </c>
       <c r="G5" s="9" t="inlineStr">
         <is>
-          <t>Grace Kwon</t>
+          <t>Hannah Zhang</t>
         </is>
       </c>
       <c r="J5" s="11" t="inlineStr">
@@ -751,31 +751,31 @@
           <t>Nathanael Wang</t>
         </is>
       </c>
-      <c r="L5" s="7" t="inlineStr">
-        <is>
-          <t>Jane Yoo</t>
+      <c r="L5" s="9" t="inlineStr">
+        <is>
+          <t>Taeho Choe</t>
         </is>
       </c>
       <c r="M5" s="9" t="inlineStr">
         <is>
-          <t>Taeho Choe</t>
+          <t>Rachel Kim</t>
         </is>
       </c>
       <c r="N5" s="9" t="inlineStr">
         <is>
-          <t>Daniel Kuo</t>
+          <t xml:space="preserve">Grace Sowon Park </t>
         </is>
       </c>
       <c r="O5" s="6" t="inlineStr">
         <is>
-          <t>Daniel Song</t>
+          <t>Emily Yang</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="D6" s="1" t="inlineStr">
         <is>
-          <t>Christina Ko</t>
+          <t>Melody Hong</t>
         </is>
       </c>
       <c r="E6" s="1" t="inlineStr">
@@ -785,12 +785,12 @@
       </c>
       <c r="F6" s="9" t="inlineStr">
         <is>
-          <t>Hannah Kim</t>
+          <t xml:space="preserve">derek liang </t>
         </is>
       </c>
       <c r="G6" s="9" t="inlineStr">
         <is>
-          <t xml:space="preserve">derek liang </t>
+          <t>Daniel Kuo</t>
         </is>
       </c>
       <c r="K6" s="1" t="inlineStr">
@@ -798,24 +798,24 @@
           <t>Grace Park</t>
         </is>
       </c>
-      <c r="L6" s="6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Daniel Kim </t>
+      <c r="L6" s="9" t="inlineStr">
+        <is>
+          <t>Kyle Hwang</t>
         </is>
       </c>
       <c r="M6" s="9" t="inlineStr">
         <is>
-          <t>Kyle Hwang</t>
+          <t>Israel Haile</t>
         </is>
       </c>
       <c r="N6" s="9" t="inlineStr">
         <is>
-          <t xml:space="preserve">Grace Sowon Park </t>
+          <t>Daniel Kuo</t>
         </is>
       </c>
       <c r="O6" s="6" t="inlineStr">
         <is>
-          <t>Emily Yang</t>
+          <t>Daniel Song</t>
         </is>
       </c>
     </row>
@@ -824,7 +824,7 @@
     <row r="9">
       <c r="C9" s="3" t="inlineStr">
         <is>
-          <t>Driver: Jonathan Mak</t>
+          <t>Driver: Jenny Sohn</t>
         </is>
       </c>
       <c r="D9" s="12" t="inlineStr">
@@ -876,7 +876,7 @@
     <row r="10">
       <c r="C10" s="6" t="inlineStr">
         <is>
-          <t>Lucy Han</t>
+          <t xml:space="preserve">Daniel Kim </t>
         </is>
       </c>
       <c r="D10" s="7" t="inlineStr">
@@ -899,19 +899,19 @@
           <t>Austin Lee</t>
         </is>
       </c>
-      <c r="K10" s="9" t="inlineStr">
-        <is>
-          <t>Ella Lu</t>
-        </is>
-      </c>
-      <c r="L10" s="7" t="inlineStr">
-        <is>
-          <t>Seojin Kwon</t>
-        </is>
-      </c>
-      <c r="M10" s="9" t="inlineStr">
-        <is>
-          <t>Elie Park</t>
+      <c r="K10" s="7" t="inlineStr">
+        <is>
+          <t>Pedro Flores-Teran</t>
+        </is>
+      </c>
+      <c r="L10" s="6" t="inlineStr">
+        <is>
+          <t>Jocelyn Youn</t>
+        </is>
+      </c>
+      <c r="M10" s="6" t="inlineStr">
+        <is>
+          <t>Gabriel Ni</t>
         </is>
       </c>
       <c r="N10" s="1" t="inlineStr">
@@ -928,7 +928,7 @@
     <row r="11">
       <c r="C11" s="6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Darius Ajebon </t>
+          <t>Emily Yang</t>
         </is>
       </c>
       <c r="E11" s="7" t="inlineStr">
@@ -938,27 +938,27 @@
       </c>
       <c r="F11" s="9" t="inlineStr">
         <is>
-          <t>Joann Jung</t>
+          <t>Jeffery Huang</t>
         </is>
       </c>
       <c r="G11" s="9" t="inlineStr">
         <is>
-          <t xml:space="preserve">Grace Sowon Park </t>
-        </is>
-      </c>
-      <c r="K11" s="9" t="inlineStr">
-        <is>
-          <t>Hyeongjun Son</t>
+          <t>Aaron duong</t>
+        </is>
+      </c>
+      <c r="K11" s="7" t="inlineStr">
+        <is>
+          <t>Shayla Nguyen</t>
         </is>
       </c>
       <c r="L11" s="7" t="inlineStr">
         <is>
-          <t>Sam Ko</t>
-        </is>
-      </c>
-      <c r="M11" s="9" t="inlineStr">
-        <is>
-          <t>Joann Jung</t>
+          <t>Seojin Kwon</t>
+        </is>
+      </c>
+      <c r="M11" s="7" t="inlineStr">
+        <is>
+          <t>April Tong</t>
         </is>
       </c>
       <c r="N11" s="1" t="inlineStr">
@@ -970,59 +970,59 @@
     <row r="12">
       <c r="C12" s="6" t="inlineStr">
         <is>
-          <t>Daniel Song</t>
+          <t xml:space="preserve">Darius Ajebon </t>
         </is>
       </c>
       <c r="F12" s="9" t="inlineStr">
         <is>
-          <t>Jiwang Lee</t>
+          <t>Elie Park</t>
         </is>
       </c>
       <c r="G12" s="9" t="inlineStr">
         <is>
-          <t>Daniel Kuo</t>
-        </is>
-      </c>
-      <c r="K12" s="7" t="inlineStr">
-        <is>
-          <t>Shayla Nguyen</t>
-        </is>
-      </c>
-      <c r="L12" s="6" t="inlineStr">
-        <is>
-          <t>Jocelyn Youn</t>
-        </is>
-      </c>
-      <c r="M12" s="7" t="inlineStr">
-        <is>
-          <t>April Tong</t>
+          <t>Hannah Kim</t>
+        </is>
+      </c>
+      <c r="K12" s="9" t="inlineStr">
+        <is>
+          <t>Elie Park</t>
+        </is>
+      </c>
+      <c r="L12" s="7" t="inlineStr">
+        <is>
+          <t>Sam Ko</t>
+        </is>
+      </c>
+      <c r="M12" s="9" t="inlineStr">
+        <is>
+          <t>Joann Jung</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="C13" s="6" t="inlineStr">
         <is>
-          <t>Jocelyn Youn</t>
+          <t>Gabriel Ni</t>
         </is>
       </c>
       <c r="F13" s="9" t="inlineStr">
         <is>
-          <t>Rachel Kim</t>
+          <t xml:space="preserve">Maya Habraken </t>
         </is>
       </c>
       <c r="G13" s="9" t="inlineStr">
         <is>
+          <t>Taeho Choe</t>
+        </is>
+      </c>
+      <c r="K13" s="9" t="inlineStr">
+        <is>
+          <t>Hyeongjun Son</t>
+        </is>
+      </c>
+      <c r="M13" s="9" t="inlineStr">
+        <is>
           <t>Ella Lu</t>
-        </is>
-      </c>
-      <c r="K13" s="7" t="inlineStr">
-        <is>
-          <t>Pedro Flores-Teran</t>
-        </is>
-      </c>
-      <c r="M13" s="6" t="inlineStr">
-        <is>
-          <t>Gabriel Ni</t>
         </is>
       </c>
     </row>
@@ -1083,7 +1083,7 @@
       </c>
       <c r="D17" s="6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Daniel Kim </t>
+          <t>Lucy Han</t>
         </is>
       </c>
       <c r="E17" s="7" t="inlineStr">
@@ -1098,12 +1098,12 @@
       </c>
       <c r="G17" s="9" t="inlineStr">
         <is>
-          <t>Kyle Hwang</t>
+          <t>Benjamin Kim</t>
         </is>
       </c>
       <c r="K17" s="9" t="inlineStr">
         <is>
-          <t>Benjamin Kim</t>
+          <t xml:space="preserve">Maya Habraken </t>
         </is>
       </c>
       <c r="L17" s="6" t="inlineStr">
@@ -1130,39 +1130,39 @@
       </c>
       <c r="F18" s="9" t="inlineStr">
         <is>
+          <t>Ella Lu</t>
+        </is>
+      </c>
+      <c r="G18" s="9" t="inlineStr">
+        <is>
+          <t>Joann Jung</t>
+        </is>
+      </c>
+      <c r="K18" s="9" t="inlineStr">
+        <is>
           <t>Hannah Zhang</t>
         </is>
       </c>
-      <c r="G18" s="9" t="inlineStr">
-        <is>
-          <t>Benjamin Kim</t>
-        </is>
-      </c>
-      <c r="K18" s="9" t="inlineStr">
-        <is>
-          <t>Hannah Zhang</t>
-        </is>
-      </c>
       <c r="O18" s="7" t="inlineStr">
         <is>
-          <t>Kaitlyn Kim (RJM 🩵) No valid driver available to assign this driver</t>
+          <t>Faith Chen (RJM 🩵) No valid driver available to assign this driver</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="F19" s="9" t="inlineStr">
         <is>
-          <t>Aaron duong</t>
+          <t>Grace Kwon</t>
         </is>
       </c>
       <c r="G19" s="9" t="inlineStr">
         <is>
-          <t>Hyeongjun Son</t>
+          <t xml:space="preserve">Grace Sowon Park </t>
         </is>
       </c>
       <c r="K19" s="9" t="inlineStr">
         <is>
-          <t xml:space="preserve">Maya Habraken </t>
+          <t>Grace Kwon</t>
         </is>
       </c>
       <c r="O19" s="7" t="inlineStr">
@@ -1174,29 +1174,29 @@
     <row r="20">
       <c r="F20" s="9" t="inlineStr">
         <is>
-          <t>Jeffery Huang</t>
+          <t>Kyle Hwang</t>
         </is>
       </c>
       <c r="G20" s="9" t="inlineStr">
         <is>
-          <t>Elie Park</t>
+          <t>Rachel Kim</t>
         </is>
       </c>
       <c r="K20" s="9" t="inlineStr">
         <is>
-          <t>Grace Kwon</t>
+          <t>Benjamin Kim</t>
         </is>
       </c>
       <c r="O20" s="7" t="inlineStr">
         <is>
-          <t>Austin Lee (RJM 🩵) No valid driver available to assign this driver</t>
+          <t>Kaitlyn Kim (RJM 🩵) No valid driver available to assign this driver</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="O21" s="7" t="inlineStr">
         <is>
-          <t>Faith Chen (RJM 🩵) No valid driver available to assign this driver</t>
+          <t>Austin Lee (RJM 🩵) No valid driver available to assign this driver</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
add button to download map on the pages
</commit_message>
<xml_diff>
--- a/api_allocate.xlsx
+++ b/api_allocate.xlsx
@@ -604,12 +604,12 @@
       </c>
       <c r="D3" s="1" t="inlineStr">
         <is>
-          <t>Grace Park</t>
+          <t>Ethan Yu</t>
         </is>
       </c>
       <c r="E3" s="1" t="inlineStr">
         <is>
-          <t>Nathanael Wang</t>
+          <t>Melody Hong</t>
         </is>
       </c>
       <c r="F3" s="7" t="inlineStr">
@@ -619,7 +619,7 @@
       </c>
       <c r="G3" s="6" t="inlineStr">
         <is>
-          <t>Emily Yang</t>
+          <t>Jocelyn Youn</t>
         </is>
       </c>
       <c r="J3" s="8" t="inlineStr">
@@ -629,27 +629,27 @@
       </c>
       <c r="K3" s="1" t="inlineStr">
         <is>
-          <t>Christina Ko</t>
+          <t>Sehyun Jung</t>
         </is>
       </c>
       <c r="L3" s="6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Darius Ajebon </t>
+          <t xml:space="preserve">Daniel Kim </t>
         </is>
       </c>
       <c r="M3" s="9" t="inlineStr">
         <is>
-          <t>Jiwang Lee</t>
+          <t xml:space="preserve">derek liang </t>
         </is>
       </c>
       <c r="N3" s="9" t="inlineStr">
         <is>
-          <t xml:space="preserve">Grace Sowon Park </t>
+          <t>Hannah Kim</t>
         </is>
       </c>
       <c r="O3" s="6" t="inlineStr">
         <is>
-          <t>Daniel Song</t>
+          <t>Lucy Han</t>
         </is>
       </c>
     </row>
@@ -666,52 +666,52 @@
       </c>
       <c r="D4" s="1" t="inlineStr">
         <is>
+          <t>Christina Ko</t>
+        </is>
+      </c>
+      <c r="E4" s="1" t="inlineStr">
+        <is>
           <t>JJ Lee</t>
         </is>
       </c>
-      <c r="E4" s="1" t="inlineStr">
-        <is>
-          <t>Ethan Yu</t>
-        </is>
-      </c>
       <c r="F4" s="9" t="inlineStr">
         <is>
-          <t>Jiwang Lee</t>
+          <t>Hyeongjun Son</t>
         </is>
       </c>
       <c r="G4" s="6" t="inlineStr">
         <is>
+          <t>Lucy Han</t>
+        </is>
+      </c>
+      <c r="J4" s="10" t="inlineStr">
+        <is>
+          <t>Lunch 💛</t>
+        </is>
+      </c>
+      <c r="K4" s="1" t="inlineStr">
+        <is>
+          <t>Grace Park</t>
+        </is>
+      </c>
+      <c r="L4" s="7" t="inlineStr">
+        <is>
+          <t>Jane Yoo</t>
+        </is>
+      </c>
+      <c r="M4" s="9" t="inlineStr">
+        <is>
+          <t>Rachel Kim</t>
+        </is>
+      </c>
+      <c r="N4" s="9" t="inlineStr">
+        <is>
+          <t>Israel Haile</t>
+        </is>
+      </c>
+      <c r="O4" s="6" t="inlineStr">
+        <is>
           <t>Daniel Song</t>
-        </is>
-      </c>
-      <c r="J4" s="10" t="inlineStr">
-        <is>
-          <t>Lunch 💛</t>
-        </is>
-      </c>
-      <c r="K4" s="1" t="inlineStr">
-        <is>
-          <t>Sehyun Jung</t>
-        </is>
-      </c>
-      <c r="L4" s="7" t="inlineStr">
-        <is>
-          <t>Jane Yoo</t>
-        </is>
-      </c>
-      <c r="M4" s="9" t="inlineStr">
-        <is>
-          <t>Taeho Choe</t>
-        </is>
-      </c>
-      <c r="N4" s="9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">derek liang </t>
-        </is>
-      </c>
-      <c r="O4" s="6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Daniel Kim </t>
         </is>
       </c>
     </row>
@@ -723,52 +723,52 @@
       </c>
       <c r="D5" s="1" t="inlineStr">
         <is>
-          <t>Joanna Wei</t>
+          <t>Nathanael Wang</t>
         </is>
       </c>
       <c r="E5" s="1" t="inlineStr">
         <is>
-          <t>Christina Ko</t>
+          <t>Grace Park</t>
         </is>
       </c>
       <c r="F5" s="9" t="inlineStr">
         <is>
-          <t>Jeffery Huang</t>
+          <t>Taeho Choe</t>
         </is>
       </c>
       <c r="G5" s="9" t="inlineStr">
         <is>
+          <t>Jiwang Lee</t>
+        </is>
+      </c>
+      <c r="J5" s="11" t="inlineStr">
+        <is>
+          <t>NLK 🧡</t>
+        </is>
+      </c>
+      <c r="K5" s="1" t="inlineStr">
+        <is>
+          <t>Nathanael Wang</t>
+        </is>
+      </c>
+      <c r="L5" s="9" t="inlineStr">
+        <is>
           <t>Kyle Hwang</t>
         </is>
       </c>
-      <c r="J5" s="11" t="inlineStr">
-        <is>
-          <t>NLK 🧡</t>
-        </is>
-      </c>
-      <c r="K5" s="1" t="inlineStr">
-        <is>
-          <t>Grace Park</t>
-        </is>
-      </c>
-      <c r="L5" s="9" t="inlineStr">
-        <is>
-          <t>Israel Haile</t>
-        </is>
-      </c>
       <c r="M5" s="9" t="inlineStr">
         <is>
-          <t>Daniel Kuo</t>
+          <t>Jiwang Lee</t>
         </is>
       </c>
       <c r="N5" s="9" t="inlineStr">
         <is>
-          <t>Hannah Kim</t>
+          <t>Taeho Choe</t>
         </is>
       </c>
       <c r="O5" s="6" t="inlineStr">
         <is>
-          <t>Emily Yang</t>
+          <t xml:space="preserve">Darius Ajebon </t>
         </is>
       </c>
     </row>
@@ -780,7 +780,7 @@
       </c>
       <c r="E6" s="1" t="inlineStr">
         <is>
-          <t>Melody Hong</t>
+          <t>Joanna Wei</t>
         </is>
       </c>
       <c r="F6" s="9" t="inlineStr">
@@ -790,17 +790,17 @@
       </c>
       <c r="G6" s="9" t="inlineStr">
         <is>
-          <t xml:space="preserve">Maya Habraken </t>
+          <t>Hannah Zhang</t>
         </is>
       </c>
       <c r="K6" s="1" t="inlineStr">
         <is>
-          <t>Nathanael Wang</t>
+          <t>Christina Ko</t>
         </is>
       </c>
       <c r="L6" s="9" t="inlineStr">
         <is>
-          <t>Rachel Kim</t>
+          <t>Daniel Kuo</t>
         </is>
       </c>
       <c r="M6" s="9" t="inlineStr">
@@ -810,12 +810,12 @@
       </c>
       <c r="N6" s="9" t="inlineStr">
         <is>
-          <t>Kyle Hwang</t>
+          <t xml:space="preserve">Grace Sowon Park </t>
         </is>
       </c>
       <c r="O6" s="6" t="inlineStr">
         <is>
-          <t>Lucy Han</t>
+          <t>Emily Yang</t>
         </is>
       </c>
     </row>
@@ -876,7 +876,7 @@
     <row r="10">
       <c r="C10" s="6" t="inlineStr">
         <is>
-          <t>helena song</t>
+          <t>Emily Yang</t>
         </is>
       </c>
       <c r="D10" s="7" t="inlineStr">
@@ -928,7 +928,7 @@
     <row r="11">
       <c r="C11" s="6" t="inlineStr">
         <is>
-          <t>Lucy Han</t>
+          <t>helena song</t>
         </is>
       </c>
       <c r="E11" s="7" t="inlineStr">
@@ -938,12 +938,12 @@
       </c>
       <c r="F11" s="9" t="inlineStr">
         <is>
+          <t>Grace Kwon</t>
+        </is>
+      </c>
+      <c r="G11" s="9" t="inlineStr">
+        <is>
           <t xml:space="preserve">Grace Sowon Park </t>
-        </is>
-      </c>
-      <c r="G11" s="9" t="inlineStr">
-        <is>
-          <t>Daniel Kuo</t>
         </is>
       </c>
       <c r="K11" s="7" t="inlineStr">
@@ -970,59 +970,59 @@
     <row r="12">
       <c r="C12" s="6" t="inlineStr">
         <is>
-          <t>Jocelyn Youn</t>
+          <t xml:space="preserve">Daniel Kim </t>
         </is>
       </c>
       <c r="F12" s="9" t="inlineStr">
         <is>
-          <t>Hyeongjun Son</t>
+          <t>Jeffery Huang</t>
         </is>
       </c>
       <c r="G12" s="9" t="inlineStr">
         <is>
+          <t>Daniel Kuo</t>
+        </is>
+      </c>
+      <c r="K12" s="9" t="inlineStr">
+        <is>
+          <t>Joann Jung</t>
+        </is>
+      </c>
+      <c r="L12" s="7" t="inlineStr">
+        <is>
+          <t>Sam Ko</t>
+        </is>
+      </c>
+      <c r="M12" s="9" t="inlineStr">
+        <is>
           <t>Elie Park</t>
-        </is>
-      </c>
-      <c r="K12" s="9" t="inlineStr">
-        <is>
-          <t>Elie Park</t>
-        </is>
-      </c>
-      <c r="L12" s="7" t="inlineStr">
-        <is>
-          <t>Sam Ko</t>
-        </is>
-      </c>
-      <c r="M12" s="9" t="inlineStr">
-        <is>
-          <t>Ella Lu</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="C13" s="6" t="inlineStr">
         <is>
-          <t>Gabriel Ni</t>
+          <t xml:space="preserve">Darius Ajebon </t>
         </is>
       </c>
       <c r="F13" s="9" t="inlineStr">
         <is>
+          <t xml:space="preserve">Maya Habraken </t>
+        </is>
+      </c>
+      <c r="G13" s="9" t="inlineStr">
+        <is>
           <t>Hannah Kim</t>
         </is>
       </c>
-      <c r="G13" s="9" t="inlineStr">
-        <is>
-          <t>Joann Jung</t>
-        </is>
-      </c>
       <c r="K13" s="9" t="inlineStr">
         <is>
-          <t>Joann Jung</t>
+          <t>Hyeongjun Son</t>
         </is>
       </c>
       <c r="M13" s="9" t="inlineStr">
         <is>
-          <t>Hyeongjun Son</t>
+          <t>Ella Lu</t>
         </is>
       </c>
     </row>
@@ -1083,7 +1083,7 @@
       </c>
       <c r="D17" s="6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Daniel Kim </t>
+          <t>Gabriel Ni</t>
         </is>
       </c>
       <c r="E17" s="7" t="inlineStr">
@@ -1098,12 +1098,12 @@
       </c>
       <c r="G17" s="9" t="inlineStr">
         <is>
-          <t>Hannah Zhang</t>
+          <t>Kyle Hwang</t>
         </is>
       </c>
       <c r="K17" s="9" t="inlineStr">
         <is>
-          <t>Hannah Zhang</t>
+          <t xml:space="preserve">Maya Habraken </t>
         </is>
       </c>
       <c r="L17" s="6" t="inlineStr">
@@ -1125,17 +1125,17 @@
     <row r="18">
       <c r="D18" s="6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Darius Ajebon </t>
+          <t>Daniel Song</t>
         </is>
       </c>
       <c r="F18" s="9" t="inlineStr">
         <is>
-          <t>Grace Kwon</t>
+          <t>Elie Park</t>
         </is>
       </c>
       <c r="G18" s="9" t="inlineStr">
         <is>
-          <t>Benjamin Kim</t>
+          <t xml:space="preserve">derek liang </t>
         </is>
       </c>
       <c r="K18" s="9" t="inlineStr">
@@ -1152,17 +1152,17 @@
     <row r="19">
       <c r="F19" s="9" t="inlineStr">
         <is>
-          <t>Taeho Choe</t>
+          <t>Israel Haile</t>
         </is>
       </c>
       <c r="G19" s="9" t="inlineStr">
         <is>
-          <t>Israel Haile</t>
+          <t>Joann Jung</t>
         </is>
       </c>
       <c r="K19" s="9" t="inlineStr">
         <is>
-          <t xml:space="preserve">Maya Habraken </t>
+          <t>Benjamin Kim</t>
         </is>
       </c>
       <c r="O19" s="7" t="inlineStr">
@@ -1174,17 +1174,17 @@
     <row r="20">
       <c r="F20" s="9" t="inlineStr">
         <is>
+          <t>Benjamin Kim</t>
+        </is>
+      </c>
+      <c r="G20" s="9" t="inlineStr">
+        <is>
           <t>Rachel Kim</t>
         </is>
       </c>
-      <c r="G20" s="9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">derek liang </t>
-        </is>
-      </c>
       <c r="K20" s="9" t="inlineStr">
         <is>
-          <t>Benjamin Kim</t>
+          <t>Hannah Zhang</t>
         </is>
       </c>
       <c r="O20" s="7" t="inlineStr">

</xml_diff>